<commit_message>
added analysis of cervCancer and spark results
</commit_message>
<xml_diff>
--- a/results_analysis/spark_vertebralColum_01_hold_02.xlsx
+++ b/results_analysis/spark_vertebralColum_01_hold_02.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\MLTool_matlab\results_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD441329-6680-4DAC-8258-CC0E428EAB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA6FD60-DC73-450C-9908-D56BE8D7FDAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_mean" sheetId="1" r:id="rId1"/>
-    <sheet name="acc_median" sheetId="7" r:id="rId2"/>
-    <sheet name="acc_best" sheetId="11" r:id="rId3"/>
-    <sheet name="nprot_best" sheetId="3" r:id="rId4"/>
-    <sheet name="nprot_mean" sheetId="8" r:id="rId5"/>
-    <sheet name="K_best" sheetId="9" r:id="rId6"/>
-    <sheet name="K_mean" sheetId="10" r:id="rId7"/>
-    <sheet name="hp_best" sheetId="12" r:id="rId8"/>
-    <sheet name="v1_v2_best" sheetId="13" r:id="rId9"/>
-    <sheet name="MCC" sheetId="14" r:id="rId10"/>
-    <sheet name="F1S" sheetId="15" r:id="rId11"/>
+    <sheet name="acc_std" sheetId="16" r:id="rId2"/>
+    <sheet name="acc_median" sheetId="7" r:id="rId3"/>
+    <sheet name="acc_best" sheetId="11" r:id="rId4"/>
+    <sheet name="nprot_best" sheetId="3" r:id="rId5"/>
+    <sheet name="nprot_mean" sheetId="8" r:id="rId6"/>
+    <sheet name="K_best" sheetId="9" r:id="rId7"/>
+    <sheet name="K_mean" sheetId="10" r:id="rId8"/>
+    <sheet name="hp_best" sheetId="12" r:id="rId9"/>
+    <sheet name="v1_v2_best" sheetId="13" r:id="rId10"/>
+    <sheet name="MCC" sheetId="14" r:id="rId11"/>
+    <sheet name="F1S" sheetId="15" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="32">
   <si>
     <t>Sparsiciation Method</t>
   </si>
@@ -128,6 +129,9 @@
   </si>
   <si>
     <t>Vertebral Column DataSet 01 - hold 02 - F1-Score (Macro-Averaged)</t>
+  </si>
+  <si>
+    <t>Vertebral Column DataSet 01 - hold 02 - Accuracy (std)</t>
   </si>
 </sst>
 </file>
@@ -995,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,6 +1924,1358 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E093FD04-CF21-4625-BBAE-D18349CAAAA7}">
+  <dimension ref="A1:S53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="63"/>
+      <c r="F3" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="63"/>
+      <c r="H3" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="63"/>
+      <c r="J3" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="63"/>
+      <c r="L3" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="63"/>
+      <c r="N3" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="63"/>
+      <c r="P3" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="64"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="27">
+        <v>2</v>
+      </c>
+      <c r="E5" s="27">
+        <v>1024.001</v>
+      </c>
+      <c r="F5" s="28">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="G5" s="27">
+        <v>1024.001</v>
+      </c>
+      <c r="H5" s="28">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="I5" s="27">
+        <v>1024.001</v>
+      </c>
+      <c r="J5" s="12">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="K5" s="27">
+        <v>1024.001</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="M5" s="27">
+        <v>1024.001</v>
+      </c>
+      <c r="N5" s="27">
+        <v>-8</v>
+      </c>
+      <c r="O5" s="27">
+        <v>1024.001</v>
+      </c>
+      <c r="P5" s="28">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="Q5" s="27">
+        <v>1024.001</v>
+      </c>
+      <c r="R5" s="28">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="S5" s="27">
+        <v>1024.001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="29">
+        <v>1</v>
+      </c>
+      <c r="E6" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="F6" s="29">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G6" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="H6" s="30">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="I6" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="J6" s="29">
+        <v>1</v>
+      </c>
+      <c r="K6" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="L6" s="30">
+        <v>3.125E-2</v>
+      </c>
+      <c r="M6" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="N6" s="29">
+        <v>-256</v>
+      </c>
+      <c r="O6" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="P6" s="31">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="Q6" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="R6" s="29">
+        <v>3.125E-2</v>
+      </c>
+      <c r="S6" s="29">
+        <v>1024.001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="29">
+        <v>4</v>
+      </c>
+      <c r="E7" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="F7" s="31">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G7" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="H7" s="29">
+        <v>8</v>
+      </c>
+      <c r="I7" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="J7" s="30">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="K7" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="L7" s="29">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="M7" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="N7" s="29">
+        <v>-1</v>
+      </c>
+      <c r="O7" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="P7" s="31">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="Q7" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="R7" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="S7" s="29">
+        <v>1024.001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="31">
+        <v>0.125</v>
+      </c>
+      <c r="E8" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="F8" s="30">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G8" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="H8" s="29">
+        <v>0.125</v>
+      </c>
+      <c r="I8" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="J8" s="19">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="K8" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="L8" s="19">
+        <v>1</v>
+      </c>
+      <c r="M8" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="N8" s="13">
+        <v>-1.953125E-3</v>
+      </c>
+      <c r="O8" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="P8" s="31">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="Q8" s="29">
+        <v>1024.001</v>
+      </c>
+      <c r="R8" s="29">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="S8" s="29">
+        <v>1024.001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="30">
+        <v>0.99</v>
+      </c>
+      <c r="E9" s="29">
+        <v>1</v>
+      </c>
+      <c r="F9" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="G9" s="29">
+        <v>1</v>
+      </c>
+      <c r="H9" s="30">
+        <v>0.9</v>
+      </c>
+      <c r="I9" s="29">
+        <v>1</v>
+      </c>
+      <c r="J9" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="K9" s="29">
+        <v>1</v>
+      </c>
+      <c r="L9" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="M9" s="29">
+        <v>1</v>
+      </c>
+      <c r="N9" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="O9" s="29">
+        <v>1</v>
+      </c>
+      <c r="P9" s="30">
+        <v>0.99</v>
+      </c>
+      <c r="Q9" s="29">
+        <v>1</v>
+      </c>
+      <c r="R9" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="S9" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="30">
+        <v>0.8</v>
+      </c>
+      <c r="E10" s="29">
+        <v>1</v>
+      </c>
+      <c r="F10" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="29">
+        <v>1</v>
+      </c>
+      <c r="H10" s="30">
+        <v>0.9</v>
+      </c>
+      <c r="I10" s="29">
+        <v>1</v>
+      </c>
+      <c r="J10" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="K10" s="29">
+        <v>1</v>
+      </c>
+      <c r="L10" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="29">
+        <v>1</v>
+      </c>
+      <c r="N10" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="O10" s="29">
+        <v>1</v>
+      </c>
+      <c r="P10" s="30">
+        <v>0.9</v>
+      </c>
+      <c r="Q10" s="29">
+        <v>1</v>
+      </c>
+      <c r="R10" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="S10" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="E11" s="29">
+        <v>1</v>
+      </c>
+      <c r="F11" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="G11" s="29">
+        <v>1</v>
+      </c>
+      <c r="H11" s="30">
+        <v>0.8</v>
+      </c>
+      <c r="I11" s="29">
+        <v>1</v>
+      </c>
+      <c r="J11" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="29">
+        <v>1</v>
+      </c>
+      <c r="L11" s="30">
+        <v>0.99</v>
+      </c>
+      <c r="M11" s="29">
+        <v>1</v>
+      </c>
+      <c r="N11" s="19">
+        <v>0.99</v>
+      </c>
+      <c r="O11" s="29">
+        <v>1</v>
+      </c>
+      <c r="P11" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="Q11" s="29">
+        <v>1</v>
+      </c>
+      <c r="R11" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="S11" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="30">
+        <v>0.8</v>
+      </c>
+      <c r="E12" s="29">
+        <v>1</v>
+      </c>
+      <c r="F12" s="30">
+        <v>0.8</v>
+      </c>
+      <c r="G12" s="29">
+        <v>1</v>
+      </c>
+      <c r="H12" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="I12" s="29">
+        <v>1</v>
+      </c>
+      <c r="J12" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="K12" s="29">
+        <v>1</v>
+      </c>
+      <c r="L12" s="30">
+        <v>0.99</v>
+      </c>
+      <c r="M12" s="29">
+        <v>1</v>
+      </c>
+      <c r="N12" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="O12" s="29">
+        <v>1</v>
+      </c>
+      <c r="P12" s="30">
+        <v>0.9</v>
+      </c>
+      <c r="Q12" s="29">
+        <v>1</v>
+      </c>
+      <c r="R12" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="S12" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="29">
+        <v>1</v>
+      </c>
+      <c r="E13" s="29">
+        <v>1024.0009765625</v>
+      </c>
+      <c r="F13" s="13">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="G13" s="29">
+        <v>256.0009765625</v>
+      </c>
+      <c r="H13" s="31">
+        <v>3.125E-2</v>
+      </c>
+      <c r="I13" s="29">
+        <v>32.0009765625</v>
+      </c>
+      <c r="J13" s="13">
+        <v>6.25E-2</v>
+      </c>
+      <c r="K13" s="29">
+        <v>8.0009765625</v>
+      </c>
+      <c r="L13" s="19">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="M13" s="29">
+        <v>16.0009765625</v>
+      </c>
+      <c r="N13" s="29">
+        <v>2</v>
+      </c>
+      <c r="O13" s="29">
+        <v>4.0009765625</v>
+      </c>
+      <c r="P13" s="31">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="Q13" s="29">
+        <v>1024.0009765625</v>
+      </c>
+      <c r="R13" s="13">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="S13" s="13">
+        <v>1.66015625E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="29">
+        <v>2</v>
+      </c>
+      <c r="E14" s="29">
+        <v>4.0009765625</v>
+      </c>
+      <c r="F14" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="19">
+        <v>0.5009765625</v>
+      </c>
+      <c r="H14" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="29">
+        <v>512.0009765625</v>
+      </c>
+      <c r="J14" s="31">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="K14" s="29">
+        <v>1.0009765625</v>
+      </c>
+      <c r="L14" s="13">
+        <v>0.125</v>
+      </c>
+      <c r="M14" s="29">
+        <v>256.0009765625</v>
+      </c>
+      <c r="N14" s="29">
+        <v>4</v>
+      </c>
+      <c r="O14" s="29">
+        <v>512.0009765625</v>
+      </c>
+      <c r="P14" s="31">
+        <v>3.125E-2</v>
+      </c>
+      <c r="Q14" s="29">
+        <v>128.0009765625</v>
+      </c>
+      <c r="R14" s="31">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="S14" s="29">
+        <v>128.0009765625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="29">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="E15" s="13">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="F15" s="29">
+        <v>32</v>
+      </c>
+      <c r="G15" s="30">
+        <v>8.7890625E-3</v>
+      </c>
+      <c r="H15" s="30">
+        <v>3.125E-2</v>
+      </c>
+      <c r="I15" s="30">
+        <v>1.66015625E-2</v>
+      </c>
+      <c r="J15" s="29">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="K15" s="13">
+        <v>6.34765625E-2</v>
+      </c>
+      <c r="L15" s="29">
+        <v>0.25</v>
+      </c>
+      <c r="M15" s="29">
+        <v>3.22265625E-2</v>
+      </c>
+      <c r="N15" s="29">
+        <v>2</v>
+      </c>
+      <c r="O15" s="13">
+        <v>8.7890625E-3</v>
+      </c>
+      <c r="P15" s="29">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="29">
+        <v>1024.0009765625</v>
+      </c>
+      <c r="R15" s="29">
+        <v>512</v>
+      </c>
+      <c r="S15" s="29">
+        <v>128.0009765625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="29">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="E16" s="29">
+        <v>4.0009765625</v>
+      </c>
+      <c r="F16" s="29">
+        <v>4</v>
+      </c>
+      <c r="G16" s="13">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="H16" s="13">
+        <v>6.25E-2</v>
+      </c>
+      <c r="I16" s="29">
+        <v>2.0009765625</v>
+      </c>
+      <c r="J16" s="29">
+        <v>64</v>
+      </c>
+      <c r="K16" s="29">
+        <v>1.66015625E-2</v>
+      </c>
+      <c r="L16" s="29">
+        <v>1024</v>
+      </c>
+      <c r="M16" s="29">
+        <v>1.66015625E-2</v>
+      </c>
+      <c r="N16" s="29">
+        <v>4</v>
+      </c>
+      <c r="O16" s="29">
+        <v>16.0009765625</v>
+      </c>
+      <c r="P16" s="29">
+        <v>16</v>
+      </c>
+      <c r="Q16" s="30">
+        <v>0.2509765625</v>
+      </c>
+      <c r="R16" s="29">
+        <v>128</v>
+      </c>
+      <c r="S16" s="29">
+        <v>64.0009765625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="29">
+        <v>4</v>
+      </c>
+      <c r="E17" s="29">
+        <v>256.0009765625</v>
+      </c>
+      <c r="F17" s="29">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G17" s="29">
+        <v>8.0009765625</v>
+      </c>
+      <c r="H17" s="31">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="I17" s="29">
+        <v>1.0009765625</v>
+      </c>
+      <c r="J17" s="29">
+        <v>1</v>
+      </c>
+      <c r="K17" s="29">
+        <v>4.0009765625</v>
+      </c>
+      <c r="L17" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="M17" s="19">
+        <v>1.0009765625</v>
+      </c>
+      <c r="N17" s="13">
+        <v>-3.125E-2</v>
+      </c>
+      <c r="O17" s="13">
+        <v>-2.9296875E-3</v>
+      </c>
+      <c r="P17" s="31">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q17" s="29">
+        <v>128.0009765625</v>
+      </c>
+      <c r="R17" s="29">
+        <v>256</v>
+      </c>
+      <c r="S17" s="29">
+        <v>1024.0009765625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="29">
+        <v>2</v>
+      </c>
+      <c r="E18" s="29">
+        <v>512.0009765625</v>
+      </c>
+      <c r="F18" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="G18" s="29">
+        <v>512.0009765625</v>
+      </c>
+      <c r="H18" s="31">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="I18" s="29">
+        <v>0.5009765625</v>
+      </c>
+      <c r="J18" s="29">
+        <v>16</v>
+      </c>
+      <c r="K18" s="29">
+        <v>128.0009765625</v>
+      </c>
+      <c r="L18" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="M18" s="29">
+        <v>32.0009765625</v>
+      </c>
+      <c r="N18" s="29">
+        <v>-128</v>
+      </c>
+      <c r="O18" s="29">
+        <v>-31.9990234375</v>
+      </c>
+      <c r="P18" s="13">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q18" s="29">
+        <v>0.2509765625</v>
+      </c>
+      <c r="R18" s="31">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="S18" s="29">
+        <v>1.66015625E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="13">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="E19" s="29">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="F19" s="13">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="G19" s="29">
+        <v>64.0009765625</v>
+      </c>
+      <c r="H19" s="31">
+        <v>6.25E-2</v>
+      </c>
+      <c r="I19" s="29">
+        <v>32.0009765625</v>
+      </c>
+      <c r="J19" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="K19" s="29">
+        <v>32.0009765625</v>
+      </c>
+      <c r="L19" s="31">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="M19" s="13">
+        <v>0.1259765625</v>
+      </c>
+      <c r="N19" s="29">
+        <v>-32</v>
+      </c>
+      <c r="O19" s="13">
+        <v>-6.8359375E-3</v>
+      </c>
+      <c r="P19" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="Q19" s="29">
+        <v>2.0009765625</v>
+      </c>
+      <c r="R19" s="31">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="S19" s="29">
+        <v>256.0009765625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="E20" s="29">
+        <v>32.0009765625</v>
+      </c>
+      <c r="F20" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="19">
+        <v>4.0009765625</v>
+      </c>
+      <c r="H20" s="29">
+        <v>8</v>
+      </c>
+      <c r="I20" s="29">
+        <v>32.0009765625</v>
+      </c>
+      <c r="J20" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="K20" s="29">
+        <v>32.0009765625</v>
+      </c>
+      <c r="L20" s="31">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="M20" s="13">
+        <v>4.8828125E-3</v>
+      </c>
+      <c r="N20" s="29">
+        <v>-256</v>
+      </c>
+      <c r="O20" s="13">
+        <v>-9.765625E-4</v>
+      </c>
+      <c r="P20" s="13">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="Q20" s="19">
+        <v>0.5009765625</v>
+      </c>
+      <c r="R20" s="31">
+        <v>3.125E-2</v>
+      </c>
+      <c r="S20" s="13">
+        <v>3.22265625E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="11"/>
+    </row>
+    <row r="37" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+    </row>
+    <row r="38" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+    </row>
+    <row r="39" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+    </row>
+    <row r="40" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+    </row>
+    <row r="41" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+    </row>
+    <row r="42" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+    </row>
+    <row r="43" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+    </row>
+    <row r="44" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+      <c r="R44" s="10"/>
+    </row>
+    <row r="45" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="10"/>
+    </row>
+    <row r="46" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
+      <c r="R46" s="10"/>
+    </row>
+    <row r="47" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10"/>
+      <c r="R47" s="10"/>
+    </row>
+    <row r="48" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+      <c r="N48" s="10"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="10"/>
+      <c r="R48" s="10"/>
+    </row>
+    <row r="49" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+      <c r="N49" s="10"/>
+      <c r="O49" s="10"/>
+      <c r="P49" s="10"/>
+      <c r="Q49" s="10"/>
+      <c r="R49" s="10"/>
+    </row>
+    <row r="50" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
+      <c r="R50" s="10"/>
+    </row>
+    <row r="51" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
+      <c r="R51" s="10"/>
+    </row>
+    <row r="52" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+      <c r="L52" s="10"/>
+      <c r="M52" s="10"/>
+      <c r="N52" s="10"/>
+      <c r="O52" s="10"/>
+      <c r="P52" s="10"/>
+      <c r="Q52" s="10"/>
+      <c r="R52" s="10"/>
+    </row>
+    <row r="53" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="10"/>
+      <c r="N53" s="10"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="10"/>
+      <c r="Q53" s="10"/>
+      <c r="R53" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8065C56F-AEED-4D36-9CB5-AF6203A45422}">
   <dimension ref="A1:K20"/>
   <sheetViews>
@@ -2522,7 +3878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF1E589-1659-439B-B1DA-4F9E028A9755}">
   <dimension ref="A1:K20"/>
   <sheetViews>
@@ -3126,6 +4482,609 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4400333C-559F-4C47-B054-9FD658B96BF7}">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="52">
+        <v>7.1289232346677098E-2</v>
+      </c>
+      <c r="E5" s="12">
+        <v>6.4076559082685502E-2</v>
+      </c>
+      <c r="F5" s="12">
+        <v>5.1493290311305999E-2</v>
+      </c>
+      <c r="G5" s="12">
+        <v>6.8757441194447599E-2</v>
+      </c>
+      <c r="H5" s="12">
+        <v>7.2539702598844499E-2</v>
+      </c>
+      <c r="I5" s="12">
+        <v>4.88297816944126E-2</v>
+      </c>
+      <c r="J5" s="12">
+        <v>4.92619700316234E-2</v>
+      </c>
+      <c r="K5" s="53">
+        <v>5.4593355597590702E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="54">
+        <v>4.2950973989807198E-2</v>
+      </c>
+      <c r="E6" s="13">
+        <v>7.7712507505501405E-2</v>
+      </c>
+      <c r="F6" s="13">
+        <v>5.6716961849039398E-2</v>
+      </c>
+      <c r="G6" s="13">
+        <v>4.9612778417199403E-2</v>
+      </c>
+      <c r="H6" s="13">
+        <v>6.7854678515837902E-2</v>
+      </c>
+      <c r="I6" s="13">
+        <v>3.9653954655023201E-2</v>
+      </c>
+      <c r="J6" s="13">
+        <v>6.3157742604681294E-2</v>
+      </c>
+      <c r="K6" s="15">
+        <v>9.0255707166340099E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="54">
+        <v>3.74032841525292E-2</v>
+      </c>
+      <c r="E7" s="13">
+        <v>8.8385963069062004E-2</v>
+      </c>
+      <c r="F7" s="13">
+        <v>7.2787218754661001E-2</v>
+      </c>
+      <c r="G7" s="13">
+        <v>6.2493174817787399E-2</v>
+      </c>
+      <c r="H7" s="13">
+        <v>5.4168130429570097E-2</v>
+      </c>
+      <c r="I7" s="13">
+        <v>0.19351187761324901</v>
+      </c>
+      <c r="J7" s="13">
+        <v>5.3415841678169602E-2</v>
+      </c>
+      <c r="K7" s="15">
+        <v>5.1142821453009198E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="55">
+        <v>6.3512706618886597E-2</v>
+      </c>
+      <c r="E8" s="14">
+        <v>8.0177857558310806E-2</v>
+      </c>
+      <c r="F8" s="14">
+        <v>5.2297824994899003E-2</v>
+      </c>
+      <c r="G8" s="14">
+        <v>7.1872513527016402E-2</v>
+      </c>
+      <c r="H8" s="14">
+        <v>5.3835077721917098E-2</v>
+      </c>
+      <c r="I8" s="14">
+        <v>7.44623116769772E-2</v>
+      </c>
+      <c r="J8" s="14">
+        <v>4.2181370236343399E-2</v>
+      </c>
+      <c r="K8" s="56">
+        <v>6.9906257256687601E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="57">
+        <v>3.9992676710432599E-2</v>
+      </c>
+      <c r="E9" s="58">
+        <v>4.7617671166976398E-2</v>
+      </c>
+      <c r="F9" s="58">
+        <v>6.6757174466494401E-2</v>
+      </c>
+      <c r="G9" s="58">
+        <v>8.5090541796266198E-2</v>
+      </c>
+      <c r="H9" s="58">
+        <v>2.70365909184891E-2</v>
+      </c>
+      <c r="I9" s="58">
+        <v>2.9030045492926999E-2</v>
+      </c>
+      <c r="J9" s="58">
+        <v>5.55382098022403E-2</v>
+      </c>
+      <c r="K9" s="59">
+        <v>4.88297816944126E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="54">
+        <v>6.9315697511877106E-2</v>
+      </c>
+      <c r="E10" s="13">
+        <v>5.0802579612622203E-2</v>
+      </c>
+      <c r="F10" s="13">
+        <v>5.1305836866743601E-2</v>
+      </c>
+      <c r="G10" s="13">
+        <v>4.2409174072398699E-2</v>
+      </c>
+      <c r="H10" s="13">
+        <v>5.1493290311305999E-2</v>
+      </c>
+      <c r="I10" s="13">
+        <v>3.8336177654827101E-2</v>
+      </c>
+      <c r="J10" s="13">
+        <v>4.4709580299677899E-2</v>
+      </c>
+      <c r="K10" s="15">
+        <v>7.4367361724897593E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="54">
+        <v>5.2248672892879003E-2</v>
+      </c>
+      <c r="E11" s="13">
+        <v>3.4172577595850899E-2</v>
+      </c>
+      <c r="F11" s="13">
+        <v>4.9157546024354702E-2</v>
+      </c>
+      <c r="G11" s="13">
+        <v>4.2409174072398699E-2</v>
+      </c>
+      <c r="H11" s="13">
+        <v>5.1989861976971301E-2</v>
+      </c>
+      <c r="I11" s="13">
+        <v>5.0192010656445303E-2</v>
+      </c>
+      <c r="J11" s="13">
+        <v>4.20440954799002E-2</v>
+      </c>
+      <c r="K11" s="15">
+        <v>7.7248251119183903E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="55">
+        <v>5.9210341315503102E-2</v>
+      </c>
+      <c r="E12" s="14">
+        <v>4.0566763632748103E-2</v>
+      </c>
+      <c r="F12" s="14">
+        <v>3.7334528057347001E-2</v>
+      </c>
+      <c r="G12" s="14">
+        <v>4.0566763632748103E-2</v>
+      </c>
+      <c r="H12" s="14">
+        <v>4.93531597937161E-2</v>
+      </c>
+      <c r="I12" s="14">
+        <v>4.0232875126601501E-2</v>
+      </c>
+      <c r="J12" s="14">
+        <v>4.6401583749626503E-2</v>
+      </c>
+      <c r="K12" s="56">
+        <v>4.3144951930621199E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="57">
+        <v>6.0071941214668099E-2</v>
+      </c>
+      <c r="E13" s="58">
+        <v>2.7036590918488999E-2</v>
+      </c>
+      <c r="F13" s="58">
+        <v>3.6552111208550397E-2</v>
+      </c>
+      <c r="G13" s="58">
+        <v>5.6262127226806E-2</v>
+      </c>
+      <c r="H13" s="58">
+        <v>6.2534275233159603E-2</v>
+      </c>
+      <c r="I13" s="58">
+        <v>4.9457170783255497E-2</v>
+      </c>
+      <c r="J13" s="58">
+        <v>2.0401791355925E-2</v>
+      </c>
+      <c r="K13" s="59">
+        <v>5.6044787710078398E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="54">
+        <v>4.5408098420501503E-2</v>
+      </c>
+      <c r="E14" s="13">
+        <v>4.8100839166654599E-2</v>
+      </c>
+      <c r="F14" s="13">
+        <v>6.2862111163852999E-2</v>
+      </c>
+      <c r="G14" s="13">
+        <v>5.2920512760693199E-2</v>
+      </c>
+      <c r="H14" s="13">
+        <v>4.1567790339581398E-2</v>
+      </c>
+      <c r="I14" s="13">
+        <v>5.3835077721917098E-2</v>
+      </c>
+      <c r="J14" s="13">
+        <v>4.1798938314303202E-2</v>
+      </c>
+      <c r="K14" s="15">
+        <v>4.3736411357079903E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="54">
+        <v>5.9588824202495803E-2</v>
+      </c>
+      <c r="E15" s="13">
+        <v>5.2725951393357097E-2</v>
+      </c>
+      <c r="F15" s="13">
+        <v>5.1989861976971301E-2</v>
+      </c>
+      <c r="G15" s="13">
+        <v>4.4203881271170899E-2</v>
+      </c>
+      <c r="H15" s="13">
+        <v>5.4839880981704697E-2</v>
+      </c>
+      <c r="I15" s="13">
+        <v>6.5071287271169703E-2</v>
+      </c>
+      <c r="J15" s="13">
+        <v>5.4073181836978103E-2</v>
+      </c>
+      <c r="K15" s="15">
+        <v>5.57690429242578E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="55">
+        <v>4.6470746977384798E-2</v>
+      </c>
+      <c r="E16" s="14">
+        <v>6.8043741792598103E-2</v>
+      </c>
+      <c r="F16" s="14">
+        <v>6.0572416270330103E-2</v>
+      </c>
+      <c r="G16" s="14">
+        <v>4.0056870454332601E-2</v>
+      </c>
+      <c r="H16" s="14">
+        <v>3.6358292911586397E-2</v>
+      </c>
+      <c r="I16" s="14">
+        <v>6.0868615671265301E-2</v>
+      </c>
+      <c r="J16" s="14">
+        <v>7.5660357287218705E-2</v>
+      </c>
+      <c r="K16" s="56">
+        <v>5.1742171849802399E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="57">
+        <v>3.7745185998281798E-2</v>
+      </c>
+      <c r="E17" s="58">
+        <v>4.3025684385441201E-2</v>
+      </c>
+      <c r="F17" s="58">
+        <v>6.3350684144188402E-2</v>
+      </c>
+      <c r="G17" s="58">
+        <v>6.9768293322616498E-2</v>
+      </c>
+      <c r="H17" s="58">
+        <v>6.04450293443234E-2</v>
+      </c>
+      <c r="I17" s="58">
+        <v>4.0056870454332601E-2</v>
+      </c>
+      <c r="J17" s="58">
+        <v>6.9139404039523705E-2</v>
+      </c>
+      <c r="K17" s="59">
+        <v>5.2689391154549799E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="54">
+        <v>7.5728244566275305E-2</v>
+      </c>
+      <c r="E18" s="13">
+        <v>3.9653954655023201E-2</v>
+      </c>
+      <c r="F18" s="13">
+        <v>5.8851256635910502E-2</v>
+      </c>
+      <c r="G18" s="13">
+        <v>6.3147571456760504E-2</v>
+      </c>
+      <c r="H18" s="13">
+        <v>5.3114361441842901E-2</v>
+      </c>
+      <c r="I18" s="13">
+        <v>6.07101171407919E-2</v>
+      </c>
+      <c r="J18" s="13">
+        <v>7.3594625191171895E-2</v>
+      </c>
+      <c r="K18" s="15">
+        <v>6.5347097778226906E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="54">
+        <v>6.06254151572478E-2</v>
+      </c>
+      <c r="E19" s="13">
+        <v>7.5388196846651795E-2</v>
+      </c>
+      <c r="F19" s="13">
+        <v>6.1498524987891698E-2</v>
+      </c>
+      <c r="G19" s="13">
+        <v>6.0029154926323401E-2</v>
+      </c>
+      <c r="H19" s="13">
+        <v>5.0549072144271699E-2</v>
+      </c>
+      <c r="I19" s="13">
+        <v>4.9729164607568502E-2</v>
+      </c>
+      <c r="J19" s="13">
+        <v>5.9771794020160397E-2</v>
+      </c>
+      <c r="K19" s="15">
+        <v>6.1831852768022499E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="55">
+        <v>4.9353159793716198E-2</v>
+      </c>
+      <c r="E20" s="14">
+        <v>5.1555623332929998E-2</v>
+      </c>
+      <c r="F20" s="14">
+        <v>6.9092936258187798E-2</v>
+      </c>
+      <c r="G20" s="14">
+        <v>8.1858651891728695E-2</v>
+      </c>
+      <c r="H20" s="14">
+        <v>7.3419857371007105E-2</v>
+      </c>
+      <c r="I20" s="14">
+        <v>7.4806568305058399E-2</v>
+      </c>
+      <c r="J20" s="14">
+        <v>6.8794799220129502E-2</v>
+      </c>
+      <c r="K20" s="56">
+        <v>6.4952724244153701E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E17B74-8A06-473F-B1B4-0C752BEBC712}">
   <dimension ref="A1:K53"/>
   <sheetViews>
@@ -3895,7 +5854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4279F1E-80F5-41C1-B97A-BFBE1F0D2B01}">
   <dimension ref="A1:K53"/>
   <sheetViews>
@@ -4823,7 +6782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D980D9F8-6B96-4F95-8395-B1BF7462FEB8}">
   <dimension ref="A1:K53"/>
   <sheetViews>
@@ -5593,7 +7552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D696DEA4-1C6D-43BD-8BC6-2C617DFECF13}">
   <dimension ref="A1:K53"/>
   <sheetViews>
@@ -6363,7 +8322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40056-F547-48DD-9331-37B657810592}">
   <dimension ref="A1:K53"/>
   <sheetViews>
@@ -7133,7 +9092,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5843C1-20CB-4050-94D7-D7DDEA36873C}">
   <dimension ref="A1:K53"/>
   <sheetViews>
@@ -7903,7 +9862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C6E2BB-CD7E-4FA9-A81B-F3147CB217E2}">
   <dimension ref="A1:P53"/>
   <sheetViews>
@@ -9040,1356 +10999,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E093FD04-CF21-4625-BBAE-D18349CAAAA7}">
-  <dimension ref="A1:S53"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-    </row>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="65" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="63"/>
-      <c r="F3" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="63"/>
-      <c r="H3" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="63"/>
-      <c r="J3" s="62" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="63"/>
-      <c r="L3" s="62" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="63"/>
-      <c r="N3" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" s="63"/>
-      <c r="P3" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="62" t="s">
-        <v>10</v>
-      </c>
-      <c r="S3" s="64"/>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="R4" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="S4" s="20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="27">
-        <v>2</v>
-      </c>
-      <c r="E5" s="27">
-        <v>1024.001</v>
-      </c>
-      <c r="F5" s="28">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="G5" s="27">
-        <v>1024.001</v>
-      </c>
-      <c r="H5" s="28">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="I5" s="27">
-        <v>1024.001</v>
-      </c>
-      <c r="J5" s="12">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="K5" s="27">
-        <v>1024.001</v>
-      </c>
-      <c r="L5" s="12">
-        <v>0.125</v>
-      </c>
-      <c r="M5" s="27">
-        <v>1024.001</v>
-      </c>
-      <c r="N5" s="27">
-        <v>-8</v>
-      </c>
-      <c r="O5" s="27">
-        <v>1024.001</v>
-      </c>
-      <c r="P5" s="28">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="Q5" s="27">
-        <v>1024.001</v>
-      </c>
-      <c r="R5" s="28">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="S5" s="27">
-        <v>1024.001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="29">
-        <v>1</v>
-      </c>
-      <c r="E6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="F6" s="29">
-        <v>3.125E-2</v>
-      </c>
-      <c r="G6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="H6" s="30">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="I6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="J6" s="29">
-        <v>1</v>
-      </c>
-      <c r="K6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="L6" s="30">
-        <v>3.125E-2</v>
-      </c>
-      <c r="M6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="N6" s="29">
-        <v>-256</v>
-      </c>
-      <c r="O6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="P6" s="31">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="Q6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="R6" s="29">
-        <v>3.125E-2</v>
-      </c>
-      <c r="S6" s="29">
-        <v>1024.001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="29">
-        <v>4</v>
-      </c>
-      <c r="E7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="F7" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="G7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="H7" s="29">
-        <v>8</v>
-      </c>
-      <c r="I7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="J7" s="30">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="K7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="L7" s="29">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="M7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="N7" s="29">
-        <v>-1</v>
-      </c>
-      <c r="O7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="P7" s="31">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="Q7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="R7" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="S7" s="29">
-        <v>1024.001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="31">
-        <v>0.125</v>
-      </c>
-      <c r="E8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="F8" s="30">
-        <v>3.125E-2</v>
-      </c>
-      <c r="G8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="H8" s="29">
-        <v>0.125</v>
-      </c>
-      <c r="I8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="J8" s="19">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="K8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="L8" s="19">
-        <v>1</v>
-      </c>
-      <c r="M8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="N8" s="13">
-        <v>-1.953125E-3</v>
-      </c>
-      <c r="O8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="P8" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="Q8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="R8" s="29">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="S8" s="29">
-        <v>1024.001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="E9" s="29">
-        <v>1</v>
-      </c>
-      <c r="F9" s="19">
-        <v>0.4</v>
-      </c>
-      <c r="G9" s="29">
-        <v>1</v>
-      </c>
-      <c r="H9" s="30">
-        <v>0.9</v>
-      </c>
-      <c r="I9" s="29">
-        <v>1</v>
-      </c>
-      <c r="J9" s="30">
-        <v>0.3</v>
-      </c>
-      <c r="K9" s="29">
-        <v>1</v>
-      </c>
-      <c r="L9" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="M9" s="29">
-        <v>1</v>
-      </c>
-      <c r="N9" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="O9" s="29">
-        <v>1</v>
-      </c>
-      <c r="P9" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="Q9" s="29">
-        <v>1</v>
-      </c>
-      <c r="R9" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="S9" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="30">
-        <v>0.8</v>
-      </c>
-      <c r="E10" s="29">
-        <v>1</v>
-      </c>
-      <c r="F10" s="19">
-        <v>0.8</v>
-      </c>
-      <c r="G10" s="29">
-        <v>1</v>
-      </c>
-      <c r="H10" s="30">
-        <v>0.9</v>
-      </c>
-      <c r="I10" s="29">
-        <v>1</v>
-      </c>
-      <c r="J10" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="K10" s="29">
-        <v>1</v>
-      </c>
-      <c r="L10" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="M10" s="29">
-        <v>1</v>
-      </c>
-      <c r="N10" s="30">
-        <v>0.3</v>
-      </c>
-      <c r="O10" s="29">
-        <v>1</v>
-      </c>
-      <c r="P10" s="30">
-        <v>0.9</v>
-      </c>
-      <c r="Q10" s="29">
-        <v>1</v>
-      </c>
-      <c r="R10" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="S10" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="30">
-        <v>0.3</v>
-      </c>
-      <c r="E11" s="29">
-        <v>1</v>
-      </c>
-      <c r="F11" s="30">
-        <v>0.6</v>
-      </c>
-      <c r="G11" s="29">
-        <v>1</v>
-      </c>
-      <c r="H11" s="30">
-        <v>0.8</v>
-      </c>
-      <c r="I11" s="29">
-        <v>1</v>
-      </c>
-      <c r="J11" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="K11" s="29">
-        <v>1</v>
-      </c>
-      <c r="L11" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="M11" s="29">
-        <v>1</v>
-      </c>
-      <c r="N11" s="19">
-        <v>0.99</v>
-      </c>
-      <c r="O11" s="29">
-        <v>1</v>
-      </c>
-      <c r="P11" s="30">
-        <v>0.3</v>
-      </c>
-      <c r="Q11" s="29">
-        <v>1</v>
-      </c>
-      <c r="R11" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="S11" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="30">
-        <v>0.8</v>
-      </c>
-      <c r="E12" s="29">
-        <v>1</v>
-      </c>
-      <c r="F12" s="30">
-        <v>0.8</v>
-      </c>
-      <c r="G12" s="29">
-        <v>1</v>
-      </c>
-      <c r="H12" s="30">
-        <v>0.2</v>
-      </c>
-      <c r="I12" s="29">
-        <v>1</v>
-      </c>
-      <c r="J12" s="30">
-        <v>0.01</v>
-      </c>
-      <c r="K12" s="29">
-        <v>1</v>
-      </c>
-      <c r="L12" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="M12" s="29">
-        <v>1</v>
-      </c>
-      <c r="N12" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="O12" s="29">
-        <v>1</v>
-      </c>
-      <c r="P12" s="30">
-        <v>0.9</v>
-      </c>
-      <c r="Q12" s="29">
-        <v>1</v>
-      </c>
-      <c r="R12" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="S12" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-      <c r="D13" s="29">
-        <v>1</v>
-      </c>
-      <c r="E13" s="29">
-        <v>1024.0009765625</v>
-      </c>
-      <c r="F13" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="G13" s="29">
-        <v>256.0009765625</v>
-      </c>
-      <c r="H13" s="31">
-        <v>3.125E-2</v>
-      </c>
-      <c r="I13" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="J13" s="13">
-        <v>6.25E-2</v>
-      </c>
-      <c r="K13" s="29">
-        <v>8.0009765625</v>
-      </c>
-      <c r="L13" s="19">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="M13" s="29">
-        <v>16.0009765625</v>
-      </c>
-      <c r="N13" s="29">
-        <v>2</v>
-      </c>
-      <c r="O13" s="29">
-        <v>4.0009765625</v>
-      </c>
-      <c r="P13" s="31">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="Q13" s="29">
-        <v>1024.0009765625</v>
-      </c>
-      <c r="R13" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="S13" s="13">
-        <v>1.66015625E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="C14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="29">
-        <v>2</v>
-      </c>
-      <c r="E14" s="29">
-        <v>4.0009765625</v>
-      </c>
-      <c r="F14" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="G14" s="19">
-        <v>0.5009765625</v>
-      </c>
-      <c r="H14" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="I14" s="29">
-        <v>512.0009765625</v>
-      </c>
-      <c r="J14" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="K14" s="29">
-        <v>1.0009765625</v>
-      </c>
-      <c r="L14" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="M14" s="29">
-        <v>256.0009765625</v>
-      </c>
-      <c r="N14" s="29">
-        <v>4</v>
-      </c>
-      <c r="O14" s="29">
-        <v>512.0009765625</v>
-      </c>
-      <c r="P14" s="31">
-        <v>3.125E-2</v>
-      </c>
-      <c r="Q14" s="29">
-        <v>128.0009765625</v>
-      </c>
-      <c r="R14" s="31">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="S14" s="29">
-        <v>128.0009765625</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="29">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="E15" s="13">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="F15" s="29">
-        <v>32</v>
-      </c>
-      <c r="G15" s="30">
-        <v>8.7890625E-3</v>
-      </c>
-      <c r="H15" s="30">
-        <v>3.125E-2</v>
-      </c>
-      <c r="I15" s="30">
-        <v>1.66015625E-2</v>
-      </c>
-      <c r="J15" s="29">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="K15" s="13">
-        <v>6.34765625E-2</v>
-      </c>
-      <c r="L15" s="29">
-        <v>0.25</v>
-      </c>
-      <c r="M15" s="29">
-        <v>3.22265625E-2</v>
-      </c>
-      <c r="N15" s="29">
-        <v>2</v>
-      </c>
-      <c r="O15" s="13">
-        <v>8.7890625E-3</v>
-      </c>
-      <c r="P15" s="29">
-        <v>4</v>
-      </c>
-      <c r="Q15" s="29">
-        <v>1024.0009765625</v>
-      </c>
-      <c r="R15" s="29">
-        <v>512</v>
-      </c>
-      <c r="S15" s="29">
-        <v>128.0009765625</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="29">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="E16" s="29">
-        <v>4.0009765625</v>
-      </c>
-      <c r="F16" s="29">
-        <v>4</v>
-      </c>
-      <c r="G16" s="13">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="H16" s="13">
-        <v>6.25E-2</v>
-      </c>
-      <c r="I16" s="29">
-        <v>2.0009765625</v>
-      </c>
-      <c r="J16" s="29">
-        <v>64</v>
-      </c>
-      <c r="K16" s="29">
-        <v>1.66015625E-2</v>
-      </c>
-      <c r="L16" s="29">
-        <v>1024</v>
-      </c>
-      <c r="M16" s="29">
-        <v>1.66015625E-2</v>
-      </c>
-      <c r="N16" s="29">
-        <v>4</v>
-      </c>
-      <c r="O16" s="29">
-        <v>16.0009765625</v>
-      </c>
-      <c r="P16" s="29">
-        <v>16</v>
-      </c>
-      <c r="Q16" s="30">
-        <v>0.2509765625</v>
-      </c>
-      <c r="R16" s="29">
-        <v>128</v>
-      </c>
-      <c r="S16" s="29">
-        <v>64.0009765625</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="29">
-        <v>4</v>
-      </c>
-      <c r="E17" s="29">
-        <v>256.0009765625</v>
-      </c>
-      <c r="F17" s="29">
-        <v>6.25E-2</v>
-      </c>
-      <c r="G17" s="29">
-        <v>8.0009765625</v>
-      </c>
-      <c r="H17" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="I17" s="29">
-        <v>1.0009765625</v>
-      </c>
-      <c r="J17" s="29">
-        <v>1</v>
-      </c>
-      <c r="K17" s="29">
-        <v>4.0009765625</v>
-      </c>
-      <c r="L17" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="M17" s="19">
-        <v>1.0009765625</v>
-      </c>
-      <c r="N17" s="13">
-        <v>-3.125E-2</v>
-      </c>
-      <c r="O17" s="13">
-        <v>-2.9296875E-3</v>
-      </c>
-      <c r="P17" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="Q17" s="29">
-        <v>128.0009765625</v>
-      </c>
-      <c r="R17" s="29">
-        <v>256</v>
-      </c>
-      <c r="S17" s="29">
-        <v>1024.0009765625</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="29">
-        <v>2</v>
-      </c>
-      <c r="E18" s="29">
-        <v>512.0009765625</v>
-      </c>
-      <c r="F18" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="G18" s="29">
-        <v>512.0009765625</v>
-      </c>
-      <c r="H18" s="31">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="I18" s="29">
-        <v>0.5009765625</v>
-      </c>
-      <c r="J18" s="29">
-        <v>16</v>
-      </c>
-      <c r="K18" s="29">
-        <v>128.0009765625</v>
-      </c>
-      <c r="L18" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="M18" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="N18" s="29">
-        <v>-128</v>
-      </c>
-      <c r="O18" s="29">
-        <v>-31.9990234375</v>
-      </c>
-      <c r="P18" s="13">
-        <v>6.25E-2</v>
-      </c>
-      <c r="Q18" s="29">
-        <v>0.2509765625</v>
-      </c>
-      <c r="R18" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="S18" s="29">
-        <v>1.66015625E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1">
-        <v>2</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="E19" s="29">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="F19" s="13">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="G19" s="29">
-        <v>64.0009765625</v>
-      </c>
-      <c r="H19" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="I19" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="J19" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="K19" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="L19" s="31">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="M19" s="13">
-        <v>0.1259765625</v>
-      </c>
-      <c r="N19" s="29">
-        <v>-32</v>
-      </c>
-      <c r="O19" s="13">
-        <v>-6.8359375E-3</v>
-      </c>
-      <c r="P19" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="Q19" s="29">
-        <v>2.0009765625</v>
-      </c>
-      <c r="R19" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="S19" s="29">
-        <v>256.0009765625</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="E20" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="F20" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="G20" s="19">
-        <v>4.0009765625</v>
-      </c>
-      <c r="H20" s="29">
-        <v>8</v>
-      </c>
-      <c r="I20" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="J20" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="K20" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="L20" s="31">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="M20" s="13">
-        <v>4.8828125E-3</v>
-      </c>
-      <c r="N20" s="29">
-        <v>-256</v>
-      </c>
-      <c r="O20" s="13">
-        <v>-9.765625E-4</v>
-      </c>
-      <c r="P20" s="13">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="Q20" s="19">
-        <v>0.5009765625</v>
-      </c>
-      <c r="R20" s="31">
-        <v>3.125E-2</v>
-      </c>
-      <c r="S20" s="13">
-        <v>3.22265625E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
-    </row>
-    <row r="37" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-    </row>
-    <row r="38" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="10"/>
-    </row>
-    <row r="39" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-    </row>
-    <row r="40" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10"/>
-    </row>
-    <row r="41" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
-      <c r="Q41" s="10"/>
-      <c r="R41" s="10"/>
-    </row>
-    <row r="42" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="10"/>
-      <c r="R42" s="10"/>
-    </row>
-    <row r="43" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-    </row>
-    <row r="44" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-    </row>
-    <row r="45" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="10"/>
-      <c r="K45" s="10"/>
-      <c r="L45" s="10"/>
-      <c r="M45" s="10"/>
-      <c r="N45" s="10"/>
-      <c r="O45" s="10"/>
-      <c r="P45" s="10"/>
-      <c r="Q45" s="10"/>
-      <c r="R45" s="10"/>
-    </row>
-    <row r="46" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
-      <c r="L46" s="10"/>
-      <c r="M46" s="10"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="10"/>
-      <c r="P46" s="10"/>
-      <c r="Q46" s="10"/>
-      <c r="R46" s="10"/>
-    </row>
-    <row r="47" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
-      <c r="L47" s="10"/>
-      <c r="M47" s="10"/>
-      <c r="N47" s="10"/>
-      <c r="O47" s="10"/>
-      <c r="P47" s="10"/>
-      <c r="Q47" s="10"/>
-      <c r="R47" s="10"/>
-    </row>
-    <row r="48" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-      <c r="L48" s="10"/>
-      <c r="M48" s="10"/>
-      <c r="N48" s="10"/>
-      <c r="O48" s="10"/>
-      <c r="P48" s="10"/>
-      <c r="Q48" s="10"/>
-      <c r="R48" s="10"/>
-    </row>
-    <row r="49" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-      <c r="L49" s="10"/>
-      <c r="M49" s="10"/>
-      <c r="N49" s="10"/>
-      <c r="O49" s="10"/>
-      <c r="P49" s="10"/>
-      <c r="Q49" s="10"/>
-      <c r="R49" s="10"/>
-    </row>
-    <row r="50" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
-      <c r="L50" s="10"/>
-      <c r="M50" s="10"/>
-      <c r="N50" s="10"/>
-      <c r="O50" s="10"/>
-      <c r="P50" s="10"/>
-      <c r="Q50" s="10"/>
-      <c r="R50" s="10"/>
-    </row>
-    <row r="51" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
-      <c r="K51" s="10"/>
-      <c r="L51" s="10"/>
-      <c r="M51" s="10"/>
-      <c r="N51" s="10"/>
-      <c r="O51" s="10"/>
-      <c r="P51" s="10"/>
-      <c r="Q51" s="10"/>
-      <c r="R51" s="10"/>
-    </row>
-    <row r="52" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
-      <c r="K52" s="10"/>
-      <c r="L52" s="10"/>
-      <c r="M52" s="10"/>
-      <c r="N52" s="10"/>
-      <c r="O52" s="10"/>
-      <c r="P52" s="10"/>
-      <c r="Q52" s="10"/>
-      <c r="R52" s="10"/>
-    </row>
-    <row r="53" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10"/>
-      <c r="K53" s="10"/>
-      <c r="L53" s="10"/>
-      <c r="M53" s="10"/>
-      <c r="N53" s="10"/>
-      <c r="O53" s="10"/>
-      <c r="P53" s="10"/>
-      <c r="Q53" s="10"/>
-      <c r="R53" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>